<commit_message>
LoadManager 기본 구조 추가
</commit_message>
<xml_diff>
--- a/Document/Item/Item.xlsx
+++ b/Document/Item/Item.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newmr\Desktop\Study\Unknown\Document\Item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B592876-074E-47F7-807C-2E449177D71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC2DE96-CD47-486D-ADFE-A5CCC7D021FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="2" r:id="rId1"/>
     <sheet name="BasicAddStat" sheetId="4" r:id="rId2"/>
-    <sheet name="Storage" sheetId="3" r:id="rId3"/>
+    <sheet name="BasicMulStat" sheetId="5" r:id="rId3"/>
+    <sheet name="Storage" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -213,8 +214,195 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mri New</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{F657D25B-B7CC-4409-A760-59C2452F6EBE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mri New:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Grade </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>증가시</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이전</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>등급의</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>스탯</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>증가량</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>배수</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>배수</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>^</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>등급</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>UniqueID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -764,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731530C-0039-42AC-944F-DD348182ED49}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1052,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFD4994-7B30-4537-97A9-4C5850CC400A}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1248,6 +1436,206 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7450EF3D-031E-4C57-AF18-7075EF6AD495}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.75" customWidth="1"/>
+    <col min="3" max="3" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="17.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8F92F5-C88D-40F1-850A-3F92C080C1C0}">
   <dimension ref="A1:D5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Item_BasicAddStat, Item_BasicMulStat 로드 추가
</commit_message>
<xml_diff>
--- a/Document/Item/Item.xlsx
+++ b/Document/Item/Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newmr\Desktop\Unknown\Document\Item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFADDB5-BEF1-4ABB-989C-6220CBA04075}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B238E382-4EC0-42DE-9FDB-1EDC822C3C6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3450" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3450" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item_ItemInfo" sheetId="2" r:id="rId1"/>
@@ -402,7 +402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>UniqueID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -585,6 +585,10 @@
   </si>
   <si>
     <t>byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IndexAndUniqueID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -985,9 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731530C-0039-42AC-944F-DD348182ED49}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1323,12 +1325,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFD4994-7B30-4537-97A9-4C5850CC400A}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="23.25" customWidth="1"/>
     <col min="2" max="2" width="23.75" customWidth="1"/>
     <col min="3" max="3" width="13.625" customWidth="1"/>
     <col min="5" max="5" width="15.875" customWidth="1"/>
@@ -1338,7 +1339,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>37</v>
@@ -1558,12 +1559,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7450EF3D-031E-4C57-AF18-7075EF6AD495}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="24.625" customWidth="1"/>
     <col min="2" max="2" width="23.75" customWidth="1"/>
     <col min="3" max="3" width="13.625" customWidth="1"/>
     <col min="5" max="5" width="15.875" customWidth="1"/>
@@ -1573,7 +1575,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>40</v>
@@ -1793,12 +1795,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8F92F5-C88D-40F1-850A-3F92C080C1C0}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="26.625" customWidth="1"/>
     <col min="2" max="2" width="12.75" customWidth="1"/>
     <col min="3" max="3" width="16.75" customWidth="1"/>
     <col min="4" max="4" width="12.25" customWidth="1"/>
@@ -1806,7 +1809,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
ItemInfo에 limitTime 추가, 헤더 include 부분 정리, Use Interface 추가
</commit_message>
<xml_diff>
--- a/Document/Item/Item.xlsx
+++ b/Document/Item/Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newmr\Desktop\Unknown\Document\Item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B238E382-4EC0-42DE-9FDB-1EDC822C3C6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB27D90B-B350-42BE-A5A7-EE998457DB85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3450" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item_ItemInfo" sheetId="2" r:id="rId1"/>
@@ -402,7 +402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
   <si>
     <t>UniqueID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -468,10 +468,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Potion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>None</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -589,6 +585,14 @@
   </si>
   <si>
     <t>IndexAndUniqueID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LimitTime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -987,9 +991,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731530C-0039-42AC-944F-DD348182ED49}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -999,16 +1005,17 @@
     <col min="4" max="9" width="15" style="1" customWidth="1"/>
     <col min="10" max="10" width="18.625" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.875" style="1" customWidth="1"/>
     <col min="13" max="13" width="16.25" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.375" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.625" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="1"/>
+    <col min="16" max="16" width="13.125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1020,13 +1027,13 @@
         <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
@@ -1035,78 +1042,84 @@
         <v>4</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="N2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -1135,30 +1148,33 @@
         <v>5</v>
       </c>
       <c r="J3" s="2">
-        <v>0</v>
+        <v>43200</v>
       </c>
       <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
         <v>-1</v>
       </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
       <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
         <v>100</v>
       </c>
-      <c r="N3" s="2">
-        <f t="shared" ref="N3:N4" si="0">ROUNDUP(M3/2, 0)</f>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:O4" si="0">ROUNDUP(N3/2, 0)</f>
         <v>50</v>
       </c>
-      <c r="O3" s="2">
-        <v>1</v>
-      </c>
       <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
         <f>ForReference_Storage!D3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1187,30 +1203,33 @@
         <v>5</v>
       </c>
       <c r="J4" s="2">
-        <v>1</v>
+        <v>43200</v>
       </c>
       <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
         <v>-1</v>
       </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
       <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
         <v>80</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="O4" s="2">
-        <v>1</v>
-      </c>
       <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
         <f>ForReference_Storage!D3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1221,10 +1240,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -1239,30 +1258,33 @@
         <v>5</v>
       </c>
       <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
         <v>2</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>-1</v>
       </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
       <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
         <v>3</v>
       </c>
-      <c r="N5" s="2">
-        <f>ROUNDUP(M5/2, 0)</f>
+      <c r="O5" s="2">
+        <f>ROUNDUP(N5/2, 0)</f>
         <v>2</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>1000</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <f>ForReference_Storage!D3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1270,13 +1292,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -1291,25 +1313,28 @@
         <v>5</v>
       </c>
       <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
         <v>3</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>-1</v>
       </c>
-      <c r="L6" s="2">
-        <v>0</v>
-      </c>
       <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
         <v>2</v>
       </c>
-      <c r="N6" s="2">
-        <f>ROUNDUP(M6/2, 0)</f>
-        <v>1</v>
-      </c>
       <c r="O6" s="2">
+        <f>ROUNDUP(N6/2, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="P6" s="2">
         <v>1000</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <f>ForReference_Storage!D3</f>
         <v>0</v>
       </c>
@@ -1339,72 +1364,72 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="G1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1575,72 +1600,72 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="E1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="G1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1795,7 +1820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8F92F5-C88D-40F1-850A-3F92C080C1C0}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1809,30 +1834,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
limitTime 엑셀 size_t -> long long 변경
</commit_message>
<xml_diff>
--- a/Document/Item/Item.xlsx
+++ b/Document/Item/Item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newmr\Desktop\Unknown\Document\Item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB27D90B-B350-42BE-A5A7-EE998457DB85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C3E742-3A21-4154-B9F4-A7210D48AFDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -402,7 +402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
   <si>
     <t>UniqueID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -593,6 +593,10 @@
   </si>
   <si>
     <t>LimitTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long long</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -994,7 +998,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1095,7 +1099,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
BASIC_STAT hp, attackDamage, magicDamage long long으로 변경
</commit_message>
<xml_diff>
--- a/Document/Item/Item.xlsx
+++ b/Document/Item/Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newmr\Desktop\Unknown\Document\Item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C3E742-3A21-4154-B9F4-A7210D48AFDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B834A2-60B2-4C1B-A069-34788F041BE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11160" yWindow="4650" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item_ItemInfo" sheetId="2" r:id="rId1"/>
@@ -997,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731530C-0039-42AC-944F-DD348182ED49}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -1354,7 +1354,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFD4994-7B30-4537-97A9-4C5850CC400A}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1409,16 +1411,16 @@
         <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>42</v>
@@ -1588,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7450EF3D-031E-4C57-AF18-7075EF6AD495}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1645,16 +1647,16 @@
         <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
ItemBasicMulStat 데이터 float으로 변경
</commit_message>
<xml_diff>
--- a/Document/Item/Item.xlsx
+++ b/Document/Item/Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newmr\Desktop\Unknown\Document\Item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B834A2-60B2-4C1B-A069-34788F041BE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130D3D60-A3D6-4769-8668-9C2A03602A64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="4650" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="4650" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item_ItemInfo" sheetId="2" r:id="rId1"/>
@@ -1591,7 +1591,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1647,31 +1647,31 @@
         <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1827,7 +1827,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
basicAddStatIndex size_t -> int 변경, ItemManager가 가진 테이블 unique_ptr-> shared_ptr 변경
</commit_message>
<xml_diff>
--- a/Document/Item/Item.xlsx
+++ b/Document/Item/Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newmr\Desktop\Unknown\Document\Item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130D3D60-A3D6-4769-8668-9C2A03602A64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB8AA4B-5B9E-486C-A7A3-CCF3E1BFBCA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="4650" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="4650" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item_ItemInfo" sheetId="2" r:id="rId1"/>
@@ -997,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731530C-0039-42AC-944F-DD348182ED49}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1102,7 +1102,7 @@
         <v>48</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>42</v>
@@ -1590,7 +1590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7450EF3D-031E-4C57-AF18-7075EF6AD495}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>

</xml_diff>